<commit_message>
adding total of the page
</commit_message>
<xml_diff>
--- a/src/main/resources/public/template/excel/templateRapportSubvention.xlsx
+++ b/src/main/resources/public/template/excel/templateRapportSubvention.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr checkCompatibility="1"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="480" windowWidth="13455" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="13560" yWindow="480" windowWidth="13455" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="ANNEXE RAPPORT - CMR" sheetId="4" r:id="rId1"/>
-    <sheet name="ANNEXE RAPPORT - Publics" sheetId="3" r:id="rId2"/>
+    <sheet name="ANNEXE RAPPORT - CMD" sheetId="6" r:id="rId2"/>
+    <sheet name="ANNEXE RAPPORT - LYC" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>ANNEXE au rapport</t>
   </si>
@@ -465,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -526,10 +527,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -568,12 +569,81 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D5"/>
+  </mergeCells>
+  <pageMargins left="0.78431372549019618" right="0.78431372549019618" top="0.98039215686274517" bottom="0.98039215686274517" header="0.50980392156862753" footer="0.50980392156862753"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="63" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D5"/>
   </mergeCells>
   <pageMargins left="0.78431372549019618" right="0.78431372549019618" top="0.98039215686274517" bottom="0.98039215686274517" header="0.50980392156862753" footer="0.50980392156862753"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>